<commit_message>
Download Invoice workflow completed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheva\OneDrive - Xalta Technology Services Pvt Ltd\Documents\UiPath\task\Amazon Perfomer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xalta Suyash\OneDrive - Xalta Technology Services Pvt Ltd\Documents\UiPath\Project Invoice\performer part 1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D632150F-1B87-4517-B4B3-E5BA1ABCB4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34F9931-CD33-4FB8-BE92-59CA95D4BAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -165,10 +165,13 @@
     <t>Amazon</t>
   </si>
   <si>
-    <t>FlipkartSite</t>
-  </si>
-  <si>
-    <t>https://www.flipkart.com/</t>
+    <t>OrchestratorStorageBucketName</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>OrchestratorStorageBucketFolderName</t>
   </si>
 </sst>
 </file>
@@ -227,7 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -238,7 +241,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -557,7 +559,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -640,11 +642,18 @@
       <c r="A6" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1830,12 +1839,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2809,9 +2813,6 @@
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" xr:uid="{7B76C791-2EB3-4322-BC67-6C0A6AA1921D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Send Mail to Developer and User done
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xalta Suyash\OneDrive - Xalta Technology Services Pvt Ltd\Documents\UiPath\Project Invoice\performer part 1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34F9931-CD33-4FB8-BE92-59CA95D4BAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8506BE87-9AE6-4D21-9350-62CB3088C54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -172,13 +172,67 @@
   </si>
   <si>
     <t>OrchestratorStorageBucketFolderName</t>
+  </si>
+  <si>
+    <t>SuccessEmailTempletePath</t>
+  </si>
+  <si>
+    <t>SuccessMailSendTo</t>
+  </si>
+  <si>
+    <t>suyash.shevade@xalta.tech</t>
+  </si>
+  <si>
+    <t>Templates/SuccessEmailTemplate.html</t>
+  </si>
+  <si>
+    <t>ExceptionEmailTempletePath</t>
+  </si>
+  <si>
+    <t>Templates/ErrorEmailTemplate.html</t>
+  </si>
+  <si>
+    <t>SuccessMailSubject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Success | Vendor Invoice Processing |Performare Part I | </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exception | Vendor Invoice Processing |Performare Part I | </t>
+  </si>
+  <si>
+    <t>ExceptionMailSubject</t>
+  </si>
+  <si>
+    <t>smtp.gmail.com</t>
+  </si>
+  <si>
+    <t>EmailPort</t>
+  </si>
+  <si>
+    <t>EmailFrom</t>
+  </si>
+  <si>
+    <t>shevadesuyash3@gmail.com</t>
+  </si>
+  <si>
+    <t>EmailSMTPPassword</t>
+  </si>
+  <si>
+    <t>qymn rnxx wyfa lyxs</t>
+  </si>
+  <si>
+    <t>come from assets</t>
+  </si>
+  <si>
+    <t>EmailServer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -208,13 +262,25 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -230,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -241,6 +307,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -556,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -654,15 +721,81 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1645,6 +1778,7 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Worked on write datatable to sheet workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xalta Suyash\OneDrive - Xalta Technology Services Pvt Ltd\Documents\UiPath\Project Invoice\performer part 1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://xaltatech-my.sharepoint.com/personal/kalyani_sonawane_xalta_tech/Documents/Documents/UiPath/Xalta_Task_Invoice_Processing_Performer_Part_I/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34F9931-CD33-4FB8-BE92-59CA95D4BAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{E34F9931-CD33-4FB8-BE92-59CA95D4BAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FFFD9C9-793E-46A1-85D8-861218EA08F7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="1968" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>OrchestratorStorageBucketFolderName</t>
+  </si>
+  <si>
+    <t>OutputFile_Folder_Path</t>
+  </si>
+  <si>
+    <t>HeaderDetails_ColumnName</t>
+  </si>
+  <si>
+    <t>HeaderDetails</t>
+  </si>
+  <si>
+    <t>C:\Users\KalyaniSonawane\Downloads\Output_Invoice</t>
   </si>
 </sst>
 </file>
@@ -559,15 +571,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -615,7 +627,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -627,7 +639,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -654,8 +666,22 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1656,16 +1682,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1702,7 +1728,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1713,7 +1739,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1827,7 +1853,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2823,12 +2849,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Updated Config and remove unuse workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xalta Suyash\OneDrive - Xalta Technology Services Pvt Ltd\Documents\UiPath\Project Invoice\performer part 1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8506BE87-9AE6-4D21-9350-62CB3088C54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBC7F7C-1EF3-429A-9738-8CEFC3069D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>EmailServer</t>
+  </si>
+  <si>
+    <t>OutputFile_Folder_Path</t>
+  </si>
+  <si>
+    <t>HeaderDetails_ColumnName</t>
+  </si>
+  <si>
+    <t>HeaderDetails</t>
   </si>
 </sst>
 </file>
@@ -626,7 +635,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -796,22 +805,33 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>